<commit_message>
Addition of basic summary stats...
...to CountryCodesAndMetrics.xls
</commit_message>
<xml_diff>
--- a/CountryCodesAndMetrics.xlsx
+++ b/CountryCodesAndMetrics.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\papers - active\Africa Neuroscience paper\Data\Data for upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388A7C85-9B01-4D0B-9743-2F8BAC89252C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A156EF11-9283-459B-B1CA-6FF5CEFA83BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>African Region</t>
   </si>
@@ -247,6 +255,51 @@
   </si>
   <si>
     <t>GERD per capita</t>
+  </si>
+  <si>
+    <t>Papers</t>
+  </si>
+  <si>
+    <t>MeanCitations</t>
+  </si>
+  <si>
+    <t>MeanImpact</t>
+  </si>
+  <si>
+    <t>AvdTech</t>
+  </si>
+  <si>
+    <t>Genetic</t>
+  </si>
+  <si>
+    <t>PlantUse</t>
+  </si>
+  <si>
+    <t>Topic1</t>
+  </si>
+  <si>
+    <t>Topic2</t>
+  </si>
+  <si>
+    <t>Topic3</t>
+  </si>
+  <si>
+    <t>Topic4</t>
+  </si>
+  <si>
+    <t>Topic5</t>
+  </si>
+  <si>
+    <t>Topic7</t>
+  </si>
+  <si>
+    <t>Topic8</t>
+  </si>
+  <si>
+    <t>Topic9</t>
+  </si>
+  <si>
+    <t>Topic6</t>
   </si>
 </sst>
 </file>
@@ -308,12 +361,42 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -329,68 +412,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -672,34 +755,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="20" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="24" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="24"/>
+    <col min="15" max="16" width="11" style="24" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="25" width="9.140625" style="28"/>
+    <col min="26" max="26" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="9" t="s">
@@ -720,18 +811,64 @@
       <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="K1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="12">
@@ -755,15 +892,60 @@
       <c r="J2" s="13">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="K2" s="27">
+        <v>70</v>
+      </c>
+      <c r="L2" s="23">
+        <v>16.3857</v>
+      </c>
+      <c r="M2" s="23">
+        <v>2.3904399999999999</v>
+      </c>
+      <c r="N2" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="O2" s="23">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="P2" s="23">
+        <v>8.5714299999999993E-2</v>
+      </c>
+      <c r="Q2" s="28">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="R2" s="28">
+        <v>0.114286</v>
+      </c>
+      <c r="S2" s="28">
+        <v>0.328571</v>
+      </c>
+      <c r="T2" s="28">
+        <v>2.85714E-2</v>
+      </c>
+      <c r="U2" s="28">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="V2" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="W2" s="28">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="X2" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="28">
+        <v>0.214286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>4</v>
       </c>
       <c r="D3" s="12">
@@ -787,15 +969,60 @@
       <c r="J3" s="13">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="K3" s="27">
+        <v>12</v>
+      </c>
+      <c r="L3" s="23">
+        <v>43.25</v>
+      </c>
+      <c r="M3" s="23">
+        <v>6.4985799999999996</v>
+      </c>
+      <c r="N3" s="23">
+        <v>0</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>8.3333299999999999E-2</v>
+      </c>
+      <c r="R3" s="28">
+        <v>0</v>
+      </c>
+      <c r="S3" s="28">
+        <v>0.91666700000000001</v>
+      </c>
+      <c r="T3" s="28">
+        <v>0</v>
+      </c>
+      <c r="U3" s="28">
+        <v>0</v>
+      </c>
+      <c r="V3" s="28">
+        <v>0</v>
+      </c>
+      <c r="W3" s="28">
+        <v>0</v>
+      </c>
+      <c r="X3" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>2</v>
       </c>
       <c r="D4" s="12">
@@ -819,15 +1046,60 @@
       <c r="J4" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="K4" s="27">
+        <v>15</v>
+      </c>
+      <c r="L4" s="23">
+        <v>5.5</v>
+      </c>
+      <c r="M4" s="23">
+        <v>2.00264</v>
+      </c>
+      <c r="N4" s="23">
+        <v>0</v>
+      </c>
+      <c r="O4" s="23">
+        <v>0</v>
+      </c>
+      <c r="P4" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>0</v>
+      </c>
+      <c r="R4" s="28">
+        <v>0</v>
+      </c>
+      <c r="S4" s="28">
+        <v>0.71428599999999998</v>
+      </c>
+      <c r="T4" s="28">
+        <v>7.1428599999999995E-2</v>
+      </c>
+      <c r="U4" s="28">
+        <v>0</v>
+      </c>
+      <c r="V4" s="28">
+        <v>0</v>
+      </c>
+      <c r="W4" s="28">
+        <v>0</v>
+      </c>
+      <c r="X4" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="28">
+        <v>0.214286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>5</v>
       </c>
       <c r="D5" s="12">
@@ -851,15 +1123,60 @@
       <c r="J5" s="13">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="K5" s="27">
+        <v>11</v>
+      </c>
+      <c r="L5" s="23">
+        <v>12.545500000000001</v>
+      </c>
+      <c r="M5" s="23">
+        <v>2.4051800000000001</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0</v>
+      </c>
+      <c r="O5" s="23">
+        <v>0</v>
+      </c>
+      <c r="P5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="28">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="R5" s="28">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="S5" s="28">
+        <v>0.63636400000000004</v>
+      </c>
+      <c r="T5" s="28">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="U5" s="28">
+        <v>0</v>
+      </c>
+      <c r="V5" s="28">
+        <v>0</v>
+      </c>
+      <c r="W5" s="28">
+        <v>0</v>
+      </c>
+      <c r="X5" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="28">
+        <v>9.0909100000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>2</v>
       </c>
       <c r="D6" s="12">
@@ -883,15 +1200,60 @@
       <c r="J6" s="13">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="K6" s="27">
+        <v>34</v>
+      </c>
+      <c r="L6" s="23">
+        <v>9.7647099999999991</v>
+      </c>
+      <c r="M6" s="23">
+        <v>2.75488</v>
+      </c>
+      <c r="N6" s="23">
+        <v>0</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0</v>
+      </c>
+      <c r="P6" s="23">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>2.9411799999999998E-2</v>
+      </c>
+      <c r="R6" s="28">
+        <v>8.8235300000000003E-2</v>
+      </c>
+      <c r="S6" s="28">
+        <v>0.64705900000000005</v>
+      </c>
+      <c r="T6" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="U6" s="28">
+        <v>0.117647</v>
+      </c>
+      <c r="V6" s="28">
+        <v>0</v>
+      </c>
+      <c r="W6" s="28">
+        <v>0</v>
+      </c>
+      <c r="X6" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>4</v>
       </c>
       <c r="D7" s="12">
@@ -915,15 +1277,60 @@
       <c r="J7" s="13">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="K7" s="27">
+        <v>2</v>
+      </c>
+      <c r="L7" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="M7" s="23">
+        <v>4.0019999999999998</v>
+      </c>
+      <c r="N7" s="23">
+        <v>0</v>
+      </c>
+      <c r="O7" s="23">
+        <v>0</v>
+      </c>
+      <c r="P7" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>0</v>
+      </c>
+      <c r="R7" s="28">
+        <v>0</v>
+      </c>
+      <c r="S7" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="T7" s="28">
+        <v>0</v>
+      </c>
+      <c r="U7" s="28">
+        <v>0</v>
+      </c>
+      <c r="V7" s="28">
+        <v>0</v>
+      </c>
+      <c r="W7" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="X7" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>2</v>
       </c>
       <c r="D8" s="12">
@@ -947,15 +1354,60 @@
       <c r="J8" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="K8" s="27">
+        <v>82</v>
+      </c>
+      <c r="L8" s="23">
+        <v>18.678999999999998</v>
+      </c>
+      <c r="M8" s="23">
+        <v>2.6901099999999998</v>
+      </c>
+      <c r="N8" s="23">
+        <v>2.4691399999999999E-2</v>
+      </c>
+      <c r="O8" s="23">
+        <v>0</v>
+      </c>
+      <c r="P8" s="23">
+        <v>0.296296</v>
+      </c>
+      <c r="Q8" s="28">
+        <v>2.4691399999999999E-2</v>
+      </c>
+      <c r="R8" s="28">
+        <v>0.123457</v>
+      </c>
+      <c r="S8" s="28">
+        <v>0.41975299999999999</v>
+      </c>
+      <c r="T8" s="28">
+        <v>4.9382700000000002E-2</v>
+      </c>
+      <c r="U8" s="28">
+        <v>1.2345699999999999E-2</v>
+      </c>
+      <c r="V8" s="28">
+        <v>9.8765400000000003E-2</v>
+      </c>
+      <c r="W8" s="28">
+        <v>2.4691399999999999E-2</v>
+      </c>
+      <c r="X8" s="28">
+        <v>7.4074100000000004E-2</v>
+      </c>
+      <c r="Y8" s="28">
+        <v>0.17283999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>0</v>
       </c>
       <c r="D9" s="12">
@@ -979,15 +1431,50 @@
       <c r="J9" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="K9" s="27">
+        <v>0</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="28">
+        <v>0</v>
+      </c>
+      <c r="R9" s="28">
+        <v>0</v>
+      </c>
+      <c r="S9" s="28">
+        <v>0</v>
+      </c>
+      <c r="T9" s="28">
+        <v>0</v>
+      </c>
+      <c r="U9" s="28">
+        <v>0</v>
+      </c>
+      <c r="V9" s="28">
+        <v>0</v>
+      </c>
+      <c r="W9" s="28">
+        <v>0</v>
+      </c>
+      <c r="X9" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>4</v>
       </c>
       <c r="D10" s="12">
@@ -1011,15 +1498,60 @@
       <c r="J10" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="K10" s="27">
+        <v>5</v>
+      </c>
+      <c r="L10" s="23">
+        <v>12.6</v>
+      </c>
+      <c r="M10" s="23">
+        <v>1.476</v>
+      </c>
+      <c r="N10" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="O10" s="23">
+        <v>0</v>
+      </c>
+      <c r="P10" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>0</v>
+      </c>
+      <c r="R10" s="28">
+        <v>0</v>
+      </c>
+      <c r="S10" s="28">
+        <v>1</v>
+      </c>
+      <c r="T10" s="28">
+        <v>0</v>
+      </c>
+      <c r="U10" s="28">
+        <v>0</v>
+      </c>
+      <c r="V10" s="28">
+        <v>0</v>
+      </c>
+      <c r="W10" s="28">
+        <v>0</v>
+      </c>
+      <c r="X10" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>2</v>
       </c>
       <c r="D11" s="12">
@@ -1043,15 +1575,60 @@
       <c r="J11" s="13">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="K11" s="27">
+        <v>3</v>
+      </c>
+      <c r="L11" s="23">
+        <v>37.333300000000001</v>
+      </c>
+      <c r="M11" s="23">
+        <v>3.0156700000000001</v>
+      </c>
+      <c r="N11" s="23">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="O11" s="23">
+        <v>0</v>
+      </c>
+      <c r="P11" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>0</v>
+      </c>
+      <c r="R11" s="28">
+        <v>0</v>
+      </c>
+      <c r="S11" s="28">
+        <v>0</v>
+      </c>
+      <c r="T11" s="28">
+        <v>0</v>
+      </c>
+      <c r="U11" s="28">
+        <v>0</v>
+      </c>
+      <c r="V11" s="28">
+        <v>0</v>
+      </c>
+      <c r="W11" s="28">
+        <v>0</v>
+      </c>
+      <c r="X11" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <v>0</v>
       </c>
       <c r="D12" s="12">
@@ -1075,15 +1652,60 @@
       <c r="J12" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="K12" s="27">
+        <v>2</v>
+      </c>
+      <c r="L12" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="M12" s="23">
+        <v>3.6764999999999999</v>
+      </c>
+      <c r="N12" s="23">
+        <v>0</v>
+      </c>
+      <c r="O12" s="23">
+        <v>0</v>
+      </c>
+      <c r="P12" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="28">
+        <v>0</v>
+      </c>
+      <c r="R12" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="S12" s="28">
+        <v>0</v>
+      </c>
+      <c r="T12" s="28">
+        <v>0</v>
+      </c>
+      <c r="U12" s="28">
+        <v>0</v>
+      </c>
+      <c r="V12" s="28">
+        <v>0</v>
+      </c>
+      <c r="W12" s="28">
+        <v>0</v>
+      </c>
+      <c r="X12" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>2</v>
       </c>
       <c r="D13" s="12">
@@ -1107,15 +1729,60 @@
       <c r="J13" s="13">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="K13" s="27">
+        <v>39</v>
+      </c>
+      <c r="L13" s="23">
+        <v>11.025600000000001</v>
+      </c>
+      <c r="M13" s="23">
+        <v>1.15944</v>
+      </c>
+      <c r="N13" s="23">
+        <v>0</v>
+      </c>
+      <c r="O13" s="23">
+        <v>0</v>
+      </c>
+      <c r="P13" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="28">
+        <v>0.15384600000000001</v>
+      </c>
+      <c r="R13" s="28">
+        <v>0.12820500000000001</v>
+      </c>
+      <c r="S13" s="28">
+        <v>0.461538</v>
+      </c>
+      <c r="T13" s="28">
+        <v>5.1282099999999997E-2</v>
+      </c>
+      <c r="U13" s="28">
+        <v>5.1282099999999997E-2</v>
+      </c>
+      <c r="V13" s="28">
+        <v>5.1282099999999997E-2</v>
+      </c>
+      <c r="W13" s="28">
+        <v>2.5641000000000001E-2</v>
+      </c>
+      <c r="X13" s="28">
+        <v>2.5641000000000001E-2</v>
+      </c>
+      <c r="Y13" s="28">
+        <v>5.1282099999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>4</v>
       </c>
       <c r="D14" s="12">
@@ -1136,18 +1803,63 @@
       <c r="I14" s="14">
         <v>156</v>
       </c>
-      <c r="J14" s="21">
+      <c r="J14" s="16">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="K14" s="27">
+        <v>26</v>
+      </c>
+      <c r="L14" s="23">
+        <v>26.423100000000002</v>
+      </c>
+      <c r="M14" s="23">
+        <v>4.1626899999999996</v>
+      </c>
+      <c r="N14" s="23">
+        <v>0</v>
+      </c>
+      <c r="O14" s="23">
+        <v>0</v>
+      </c>
+      <c r="P14" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="28">
+        <v>3.8461500000000003E-2</v>
+      </c>
+      <c r="R14" s="28">
+        <v>0</v>
+      </c>
+      <c r="S14" s="28">
+        <v>0.65384600000000004</v>
+      </c>
+      <c r="T14" s="28">
+        <v>0</v>
+      </c>
+      <c r="U14" s="28">
+        <v>3.8461500000000003E-2</v>
+      </c>
+      <c r="V14" s="28">
+        <v>0</v>
+      </c>
+      <c r="W14" s="28">
+        <v>0</v>
+      </c>
+      <c r="X14" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="28">
+        <v>0.269231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="5">
         <v>3</v>
       </c>
       <c r="D15" s="12">
@@ -1168,18 +1880,63 @@
       <c r="I15" s="14">
         <v>115</v>
       </c>
-      <c r="J15" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+      <c r="K15" s="27">
+        <v>1</v>
+      </c>
+      <c r="L15" s="23">
+        <v>1</v>
+      </c>
+      <c r="M15" s="23">
+        <v>0</v>
+      </c>
+      <c r="N15" s="23">
+        <v>0</v>
+      </c>
+      <c r="O15" s="23">
+        <v>0</v>
+      </c>
+      <c r="P15" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="28">
+        <v>0</v>
+      </c>
+      <c r="R15" s="28">
+        <v>0</v>
+      </c>
+      <c r="S15" s="28">
+        <v>1</v>
+      </c>
+      <c r="T15" s="28">
+        <v>0</v>
+      </c>
+      <c r="U15" s="28">
+        <v>0</v>
+      </c>
+      <c r="V15" s="28">
+        <v>0</v>
+      </c>
+      <c r="W15" s="28">
+        <v>0</v>
+      </c>
+      <c r="X15" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="5">
         <v>1</v>
       </c>
       <c r="D16" s="12">
@@ -1203,15 +1960,60 @@
       <c r="J16" s="13">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="K16" s="27">
+        <v>1507</v>
+      </c>
+      <c r="L16" s="23">
+        <v>22.648800000000001</v>
+      </c>
+      <c r="M16" s="23">
+        <v>2.33785</v>
+      </c>
+      <c r="N16" s="23">
+        <v>0.24560199999999999</v>
+      </c>
+      <c r="O16" s="23">
+        <v>2.7063600000000001E-3</v>
+      </c>
+      <c r="P16" s="23">
+        <v>4.6008100000000003E-2</v>
+      </c>
+      <c r="Q16" s="28">
+        <v>0.104195</v>
+      </c>
+      <c r="R16" s="28">
+        <v>0.123139</v>
+      </c>
+      <c r="S16" s="28">
+        <v>0.37483100000000003</v>
+      </c>
+      <c r="T16" s="28">
+        <v>4.1948600000000003E-2</v>
+      </c>
+      <c r="U16" s="28">
+        <v>2.0974300000000001E-2</v>
+      </c>
+      <c r="V16" s="28">
+        <v>8.7280099999999999E-2</v>
+      </c>
+      <c r="W16" s="28">
+        <v>1.9621099999999999E-2</v>
+      </c>
+      <c r="X16" s="28">
+        <v>2.1650900000000001E-2</v>
+      </c>
+      <c r="Y16" s="28">
+        <v>0.20635999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="5">
         <v>4</v>
       </c>
       <c r="D17" s="12">
@@ -1232,18 +2034,53 @@
       <c r="I17" s="14">
         <v>65</v>
       </c>
-      <c r="J17" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="J17" s="16">
+        <v>0</v>
+      </c>
+      <c r="K17" s="27">
+        <v>0</v>
+      </c>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="28">
+        <v>0</v>
+      </c>
+      <c r="R17" s="28">
+        <v>0</v>
+      </c>
+      <c r="S17" s="28">
+        <v>0</v>
+      </c>
+      <c r="T17" s="28">
+        <v>0</v>
+      </c>
+      <c r="U17" s="28">
+        <v>0</v>
+      </c>
+      <c r="V17" s="28">
+        <v>0</v>
+      </c>
+      <c r="W17" s="28">
+        <v>0</v>
+      </c>
+      <c r="X17" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="5">
         <v>3</v>
       </c>
       <c r="D18" s="12">
@@ -1264,18 +2101,63 @@
       <c r="I18" s="14">
         <v>138</v>
       </c>
-      <c r="J18" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="J18" s="16">
+        <v>0</v>
+      </c>
+      <c r="K18" s="27">
+        <v>1</v>
+      </c>
+      <c r="L18" s="23">
+        <v>143</v>
+      </c>
+      <c r="M18" s="23">
+        <v>3.44</v>
+      </c>
+      <c r="N18" s="23">
+        <v>0</v>
+      </c>
+      <c r="O18" s="23">
+        <v>0</v>
+      </c>
+      <c r="P18" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="28">
+        <v>0</v>
+      </c>
+      <c r="R18" s="28">
+        <v>0</v>
+      </c>
+      <c r="S18" s="28">
+        <v>0</v>
+      </c>
+      <c r="T18" s="28">
+        <v>0</v>
+      </c>
+      <c r="U18" s="28">
+        <v>0</v>
+      </c>
+      <c r="V18" s="28">
+        <v>0</v>
+      </c>
+      <c r="W18" s="28">
+        <v>0</v>
+      </c>
+      <c r="X18" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="5">
         <v>3</v>
       </c>
       <c r="D19" s="12">
@@ -1299,15 +2181,60 @@
       <c r="J19" s="13">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="K19" s="27">
+        <v>124</v>
+      </c>
+      <c r="L19" s="23">
+        <v>21.7563</v>
+      </c>
+      <c r="M19" s="23">
+        <v>2.14262</v>
+      </c>
+      <c r="N19" s="23">
+        <v>7.5630299999999998E-2</v>
+      </c>
+      <c r="O19" s="23">
+        <v>0</v>
+      </c>
+      <c r="P19" s="23">
+        <v>6.7226900000000006E-2</v>
+      </c>
+      <c r="Q19" s="28">
+        <v>0.10084</v>
+      </c>
+      <c r="R19" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="S19" s="28">
+        <v>0.27731099999999997</v>
+      </c>
+      <c r="T19" s="28">
+        <v>3.3613400000000002E-2</v>
+      </c>
+      <c r="U19" s="28">
+        <v>1.6806700000000001E-2</v>
+      </c>
+      <c r="V19" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="W19" s="28">
+        <v>0.12605</v>
+      </c>
+      <c r="X19" s="28">
+        <v>5.0420199999999998E-2</v>
+      </c>
+      <c r="Y19" s="28">
+        <v>0.27731099999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="5">
         <v>4</v>
       </c>
       <c r="D20" s="12">
@@ -1331,15 +2258,60 @@
       <c r="J20" s="13">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="K20" s="27">
+        <v>8</v>
+      </c>
+      <c r="L20" s="23">
+        <v>26.5</v>
+      </c>
+      <c r="M20" s="23">
+        <v>1.49587</v>
+      </c>
+      <c r="N20" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="O20" s="23">
+        <v>0</v>
+      </c>
+      <c r="P20" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="28">
+        <v>0</v>
+      </c>
+      <c r="R20" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="S20" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="T20" s="28">
+        <v>0</v>
+      </c>
+      <c r="U20" s="28">
+        <v>0</v>
+      </c>
+      <c r="V20" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="W20" s="28">
+        <v>0</v>
+      </c>
+      <c r="X20" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="5">
         <v>4</v>
       </c>
       <c r="D21" s="12">
@@ -1363,15 +2335,60 @@
       <c r="J21" s="13">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="K21" s="27">
+        <v>14</v>
+      </c>
+      <c r="L21" s="23">
+        <v>29.071400000000001</v>
+      </c>
+      <c r="M21" s="23">
+        <v>7.6986400000000001</v>
+      </c>
+      <c r="N21" s="23">
+        <v>0.35714299999999999</v>
+      </c>
+      <c r="O21" s="23">
+        <v>0</v>
+      </c>
+      <c r="P21" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="28">
+        <v>7.1428599999999995E-2</v>
+      </c>
+      <c r="R21" s="28">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="S21" s="28">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="T21" s="28">
+        <v>0</v>
+      </c>
+      <c r="U21" s="28">
+        <v>0</v>
+      </c>
+      <c r="V21" s="28">
+        <v>7.1428599999999995E-2</v>
+      </c>
+      <c r="W21" s="28">
+        <v>0</v>
+      </c>
+      <c r="X21" s="28">
+        <v>7.1428599999999995E-2</v>
+      </c>
+      <c r="Y21" s="28">
+        <v>0.35714299999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="5">
         <v>2</v>
       </c>
       <c r="D22" s="12">
@@ -1395,15 +2412,60 @@
       <c r="J22" s="13">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="K22" s="27">
+        <v>62</v>
+      </c>
+      <c r="L22" s="23">
+        <v>17.333300000000001</v>
+      </c>
+      <c r="M22" s="23">
+        <v>3.2475999999999998</v>
+      </c>
+      <c r="N22" s="23">
+        <v>3.3333300000000003E-2</v>
+      </c>
+      <c r="O22" s="23">
+        <v>0</v>
+      </c>
+      <c r="P22" s="23">
+        <v>0.183333</v>
+      </c>
+      <c r="Q22" s="28">
+        <v>3.3333300000000003E-2</v>
+      </c>
+      <c r="R22" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="S22" s="28">
+        <v>0.38333299999999998</v>
+      </c>
+      <c r="T22" s="28">
+        <v>0</v>
+      </c>
+      <c r="U22" s="28">
+        <v>0</v>
+      </c>
+      <c r="V22" s="28">
+        <v>0.05</v>
+      </c>
+      <c r="W22" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="X22" s="28">
+        <v>8.3333299999999999E-2</v>
+      </c>
+      <c r="Y22" s="28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="5">
         <v>2</v>
       </c>
       <c r="D23" s="12">
@@ -1424,18 +2486,63 @@
       <c r="I23" s="14">
         <v>96</v>
       </c>
-      <c r="J23" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="J23" s="16">
+        <v>0</v>
+      </c>
+      <c r="K23" s="27">
+        <v>9</v>
+      </c>
+      <c r="L23" s="23">
+        <v>2.875</v>
+      </c>
+      <c r="M23" s="23">
+        <v>0.49037500000000001</v>
+      </c>
+      <c r="N23" s="23">
+        <v>0</v>
+      </c>
+      <c r="O23" s="23">
+        <v>0</v>
+      </c>
+      <c r="P23" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="28">
+        <v>0</v>
+      </c>
+      <c r="R23" s="28">
+        <v>0</v>
+      </c>
+      <c r="S23" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="T23" s="28">
+        <v>0</v>
+      </c>
+      <c r="U23" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="V23" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="W23" s="28">
+        <v>0</v>
+      </c>
+      <c r="X23" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="5">
         <v>2</v>
       </c>
       <c r="D24" s="12">
@@ -1456,18 +2563,63 @@
       <c r="I24" s="14">
         <v>116</v>
       </c>
-      <c r="J24" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="J24" s="16">
+        <v>0</v>
+      </c>
+      <c r="K24" s="27">
+        <v>1</v>
+      </c>
+      <c r="L24" s="23">
+        <v>4</v>
+      </c>
+      <c r="M24" s="23">
+        <v>2.6</v>
+      </c>
+      <c r="N24" s="23">
+        <v>0</v>
+      </c>
+      <c r="O24" s="23">
+        <v>0</v>
+      </c>
+      <c r="P24" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="28">
+        <v>0</v>
+      </c>
+      <c r="R24" s="28">
+        <v>0</v>
+      </c>
+      <c r="S24" s="28">
+        <v>0</v>
+      </c>
+      <c r="T24" s="28">
+        <v>0</v>
+      </c>
+      <c r="U24" s="28">
+        <v>0</v>
+      </c>
+      <c r="V24" s="28">
+        <v>0</v>
+      </c>
+      <c r="W24" s="28">
+        <v>0</v>
+      </c>
+      <c r="X24" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5">
         <v>3</v>
       </c>
       <c r="D25" s="12">
@@ -1491,15 +2643,60 @@
       <c r="J25" s="13">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="K25" s="27">
+        <v>133</v>
+      </c>
+      <c r="L25" s="23">
+        <v>20.0687</v>
+      </c>
+      <c r="M25" s="23">
+        <v>2.8326099999999999</v>
+      </c>
+      <c r="N25" s="23">
+        <v>2.2900799999999999E-2</v>
+      </c>
+      <c r="O25" s="23">
+        <v>0</v>
+      </c>
+      <c r="P25" s="23">
+        <v>3.8167899999999998E-2</v>
+      </c>
+      <c r="Q25" s="28">
+        <v>6.8702299999999994E-2</v>
+      </c>
+      <c r="R25" s="28">
+        <v>0.10687000000000001</v>
+      </c>
+      <c r="S25" s="28">
+        <v>0.51908399999999999</v>
+      </c>
+      <c r="T25" s="28">
+        <v>3.8167899999999998E-2</v>
+      </c>
+      <c r="U25" s="28">
+        <v>7.63359E-3</v>
+      </c>
+      <c r="V25" s="28">
+        <v>2.2900799999999999E-2</v>
+      </c>
+      <c r="W25" s="28">
+        <v>1.52672E-2</v>
+      </c>
+      <c r="X25" s="28">
+        <v>1.52672E-2</v>
+      </c>
+      <c r="Y25" s="28">
+        <v>0.20610700000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="5">
         <v>5</v>
       </c>
       <c r="D26" s="12">
@@ -1523,15 +2720,50 @@
       <c r="J26" s="13">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="K26" s="27">
+        <v>0</v>
+      </c>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="28">
+        <v>0</v>
+      </c>
+      <c r="R26" s="28">
+        <v>0</v>
+      </c>
+      <c r="S26" s="28">
+        <v>0</v>
+      </c>
+      <c r="T26" s="28">
+        <v>0</v>
+      </c>
+      <c r="U26" s="28">
+        <v>0</v>
+      </c>
+      <c r="V26" s="28">
+        <v>0</v>
+      </c>
+      <c r="W26" s="28">
+        <v>0</v>
+      </c>
+      <c r="X26" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="5">
         <v>2</v>
       </c>
       <c r="D27" s="12">
@@ -1552,18 +2784,53 @@
       <c r="I27" s="14">
         <v>63</v>
       </c>
-      <c r="J27" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="J27" s="16">
+        <v>0</v>
+      </c>
+      <c r="K27" s="27">
+        <v>0</v>
+      </c>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="28">
+        <v>0</v>
+      </c>
+      <c r="R27" s="28">
+        <v>0</v>
+      </c>
+      <c r="S27" s="28">
+        <v>0</v>
+      </c>
+      <c r="T27" s="28">
+        <v>0</v>
+      </c>
+      <c r="U27" s="28">
+        <v>0</v>
+      </c>
+      <c r="V27" s="28">
+        <v>0</v>
+      </c>
+      <c r="W27" s="28">
+        <v>0</v>
+      </c>
+      <c r="X27" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="5">
         <v>1</v>
       </c>
       <c r="D28" s="12">
@@ -1584,18 +2851,63 @@
       <c r="I28" s="14">
         <v>157</v>
       </c>
-      <c r="J28" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="J28" s="16">
+        <v>0</v>
+      </c>
+      <c r="K28" s="27">
+        <v>17</v>
+      </c>
+      <c r="L28" s="23">
+        <v>19.470600000000001</v>
+      </c>
+      <c r="M28" s="23">
+        <v>3.4700600000000001</v>
+      </c>
+      <c r="N28" s="23">
+        <v>0</v>
+      </c>
+      <c r="O28" s="23">
+        <v>0</v>
+      </c>
+      <c r="P28" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="28">
+        <v>0.117647</v>
+      </c>
+      <c r="R28" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="S28" s="28">
+        <v>0.352941</v>
+      </c>
+      <c r="T28" s="28">
+        <v>0</v>
+      </c>
+      <c r="U28" s="28">
+        <v>0</v>
+      </c>
+      <c r="V28" s="28">
+        <v>0.17647099999999999</v>
+      </c>
+      <c r="W28" s="28">
+        <v>5.8823500000000001E-2</v>
+      </c>
+      <c r="X28" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="28">
+        <v>0.235294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="5">
         <v>3</v>
       </c>
       <c r="D29" s="12">
@@ -1619,15 +2931,60 @@
       <c r="J29" s="13">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="K29" s="27">
+        <v>30</v>
+      </c>
+      <c r="L29" s="23">
+        <v>20.045500000000001</v>
+      </c>
+      <c r="M29" s="23">
+        <v>1.41282</v>
+      </c>
+      <c r="N29" s="23">
+        <v>0</v>
+      </c>
+      <c r="O29" s="23">
+        <v>0</v>
+      </c>
+      <c r="P29" s="23">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="Q29" s="28">
+        <v>9.0909100000000007E-2</v>
+      </c>
+      <c r="R29" s="28">
+        <v>0.13636400000000001</v>
+      </c>
+      <c r="S29" s="28">
+        <v>0.63636400000000004</v>
+      </c>
+      <c r="T29" s="28">
+        <v>0</v>
+      </c>
+      <c r="U29" s="28">
+        <v>0</v>
+      </c>
+      <c r="V29" s="28">
+        <v>0</v>
+      </c>
+      <c r="W29" s="28">
+        <v>0</v>
+      </c>
+      <c r="X29" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="28">
+        <v>0.13636400000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="5">
         <v>4</v>
       </c>
       <c r="D30" s="12">
@@ -1651,15 +3008,60 @@
       <c r="J30" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="K30" s="27">
+        <v>73</v>
+      </c>
+      <c r="L30" s="23">
+        <v>30.380299999999998</v>
+      </c>
+      <c r="M30" s="23">
+        <v>4.9509400000000001</v>
+      </c>
+      <c r="N30" s="23">
+        <v>2.8169E-2</v>
+      </c>
+      <c r="O30" s="23">
+        <v>0</v>
+      </c>
+      <c r="P30" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="28">
+        <v>4.2253499999999999E-2</v>
+      </c>
+      <c r="R30" s="28">
+        <v>1.40845E-2</v>
+      </c>
+      <c r="S30" s="28">
+        <v>0.61971799999999999</v>
+      </c>
+      <c r="T30" s="28">
+        <v>0</v>
+      </c>
+      <c r="U30" s="28">
+        <v>1.40845E-2</v>
+      </c>
+      <c r="V30" s="28">
+        <v>1.40845E-2</v>
+      </c>
+      <c r="W30" s="28">
+        <v>5.6337999999999999E-2</v>
+      </c>
+      <c r="X30" s="28">
+        <v>2.8169E-2</v>
+      </c>
+      <c r="Y30" s="28">
+        <v>0.21126800000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="5">
         <v>2</v>
       </c>
       <c r="D31" s="12">
@@ -1683,15 +3085,60 @@
       <c r="J31" s="13">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="K31" s="27">
+        <v>19</v>
+      </c>
+      <c r="L31" s="23">
+        <v>8.2631599999999992</v>
+      </c>
+      <c r="M31" s="23">
+        <v>1.0215799999999999</v>
+      </c>
+      <c r="N31" s="23">
+        <v>0</v>
+      </c>
+      <c r="O31" s="23">
+        <v>0</v>
+      </c>
+      <c r="P31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="28">
+        <v>0.105263</v>
+      </c>
+      <c r="R31" s="28">
+        <v>5.2631600000000001E-2</v>
+      </c>
+      <c r="S31" s="28">
+        <v>0.68421100000000001</v>
+      </c>
+      <c r="T31" s="28">
+        <v>5.2631600000000001E-2</v>
+      </c>
+      <c r="U31" s="28">
+        <v>0</v>
+      </c>
+      <c r="V31" s="28">
+        <v>0</v>
+      </c>
+      <c r="W31" s="28">
+        <v>0</v>
+      </c>
+      <c r="X31" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="28">
+        <v>0.105263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="5">
         <v>2</v>
       </c>
       <c r="D32" s="12">
@@ -1712,18 +3159,63 @@
       <c r="I32" s="14">
         <v>127</v>
       </c>
-      <c r="J32" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="J32" s="16">
+        <v>0</v>
+      </c>
+      <c r="K32" s="27">
+        <v>4</v>
+      </c>
+      <c r="L32" s="23">
+        <v>8.25</v>
+      </c>
+      <c r="M32" s="23">
+        <v>2.5337499999999999</v>
+      </c>
+      <c r="N32" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="O32" s="23">
+        <v>0</v>
+      </c>
+      <c r="P32" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="R32" s="28">
+        <v>0</v>
+      </c>
+      <c r="S32" s="28">
+        <v>0.75</v>
+      </c>
+      <c r="T32" s="28">
+        <v>0</v>
+      </c>
+      <c r="U32" s="28">
+        <v>0</v>
+      </c>
+      <c r="V32" s="28">
+        <v>0</v>
+      </c>
+      <c r="W32" s="28">
+        <v>0</v>
+      </c>
+      <c r="X32" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="5">
         <v>0</v>
       </c>
       <c r="D33" s="12">
@@ -1747,15 +3239,60 @@
       <c r="J33" s="13">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="K33" s="27">
+        <v>7</v>
+      </c>
+      <c r="L33" s="23">
+        <v>65.428600000000003</v>
+      </c>
+      <c r="M33" s="23">
+        <v>4.4095700000000004</v>
+      </c>
+      <c r="N33" s="23">
+        <v>0</v>
+      </c>
+      <c r="O33" s="23">
+        <v>0</v>
+      </c>
+      <c r="P33" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="28">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="R33" s="28">
+        <v>0</v>
+      </c>
+      <c r="S33" s="28">
+        <v>0</v>
+      </c>
+      <c r="T33" s="28">
+        <v>0</v>
+      </c>
+      <c r="U33" s="28">
+        <v>0</v>
+      </c>
+      <c r="V33" s="28">
+        <v>0.14285700000000001</v>
+      </c>
+      <c r="W33" s="28">
+        <v>0.28571400000000002</v>
+      </c>
+      <c r="X33" s="28">
+        <v>0.42857099999999998</v>
+      </c>
+      <c r="Y33" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="5">
         <v>1</v>
       </c>
       <c r="D34" s="12">
@@ -1779,15 +3316,60 @@
       <c r="J34" s="13">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="K34" s="27">
+        <v>418</v>
+      </c>
+      <c r="L34" s="23">
+        <v>9.9902200000000008</v>
+      </c>
+      <c r="M34" s="23">
+        <v>1.681</v>
+      </c>
+      <c r="N34" s="23">
+        <v>0.16625899999999999</v>
+      </c>
+      <c r="O34" s="23">
+        <v>0</v>
+      </c>
+      <c r="P34" s="23">
+        <v>1.7114899999999999E-2</v>
+      </c>
+      <c r="Q34" s="28">
+        <v>7.3349600000000001E-2</v>
+      </c>
+      <c r="R34" s="28">
+        <v>0.15647900000000001</v>
+      </c>
+      <c r="S34" s="28">
+        <v>0.44498799999999999</v>
+      </c>
+      <c r="T34" s="28">
+        <v>4.6454799999999997E-2</v>
+      </c>
+      <c r="U34" s="28">
+        <v>1.9559900000000002E-2</v>
+      </c>
+      <c r="V34" s="28">
+        <v>0.13447400000000001</v>
+      </c>
+      <c r="W34" s="28">
+        <v>2.9339899999999999E-2</v>
+      </c>
+      <c r="X34" s="28">
+        <v>1.7114899999999999E-2</v>
+      </c>
+      <c r="Y34" s="28">
+        <v>7.8239600000000006E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="5">
         <v>3</v>
       </c>
       <c r="D35" s="12">
@@ -1811,15 +3393,60 @@
       <c r="J35" s="13">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="K35" s="27">
+        <v>21</v>
+      </c>
+      <c r="L35" s="23">
+        <v>30.8095</v>
+      </c>
+      <c r="M35" s="23">
+        <v>5.11409</v>
+      </c>
+      <c r="N35" s="23">
+        <v>0</v>
+      </c>
+      <c r="O35" s="23">
+        <v>0</v>
+      </c>
+      <c r="P35" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="28">
+        <v>9.5238100000000006E-2</v>
+      </c>
+      <c r="R35" s="28">
+        <v>0</v>
+      </c>
+      <c r="S35" s="28">
+        <v>0.52381</v>
+      </c>
+      <c r="T35" s="28">
+        <v>9.5238100000000006E-2</v>
+      </c>
+      <c r="U35" s="28">
+        <v>0</v>
+      </c>
+      <c r="V35" s="28">
+        <v>4.7619000000000002E-2</v>
+      </c>
+      <c r="W35" s="28">
+        <v>0</v>
+      </c>
+      <c r="X35" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="28">
+        <v>0.238095</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="5">
         <v>5</v>
       </c>
       <c r="D36" s="12">
@@ -1843,15 +3470,60 @@
       <c r="J36" s="13">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="K36" s="27">
+        <v>7</v>
+      </c>
+      <c r="L36" s="23">
+        <v>31.333300000000001</v>
+      </c>
+      <c r="M36" s="23">
+        <v>1.4503299999999999</v>
+      </c>
+      <c r="N36" s="23">
+        <v>0</v>
+      </c>
+      <c r="O36" s="23">
+        <v>0</v>
+      </c>
+      <c r="P36" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="28">
+        <v>0</v>
+      </c>
+      <c r="R36" s="28">
+        <v>0.16666700000000001</v>
+      </c>
+      <c r="S36" s="28">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="T36" s="28">
+        <v>0</v>
+      </c>
+      <c r="U36" s="28">
+        <v>0</v>
+      </c>
+      <c r="V36" s="28">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="W36" s="28">
+        <v>0</v>
+      </c>
+      <c r="X36" s="28">
+        <v>0.16666700000000001</v>
+      </c>
+      <c r="Y36" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="5">
         <v>2</v>
       </c>
       <c r="D37" s="12">
@@ -1872,18 +3544,63 @@
       <c r="I37" s="14">
         <v>128</v>
       </c>
-      <c r="J37" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="J37" s="16">
+        <v>0</v>
+      </c>
+      <c r="K37" s="27">
+        <v>11</v>
+      </c>
+      <c r="L37" s="23">
+        <v>33.625</v>
+      </c>
+      <c r="M37" s="23">
+        <v>1.41438</v>
+      </c>
+      <c r="N37" s="23">
+        <v>0</v>
+      </c>
+      <c r="O37" s="23">
+        <v>0</v>
+      </c>
+      <c r="P37" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="28">
+        <v>0.25</v>
+      </c>
+      <c r="R37" s="28">
+        <v>0</v>
+      </c>
+      <c r="S37" s="28">
+        <v>0.375</v>
+      </c>
+      <c r="T37" s="28">
+        <v>0.125</v>
+      </c>
+      <c r="U37" s="28">
+        <v>0</v>
+      </c>
+      <c r="V37" s="28">
+        <v>0</v>
+      </c>
+      <c r="W37" s="28">
+        <v>0</v>
+      </c>
+      <c r="X37" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="28">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="5">
         <v>2</v>
       </c>
       <c r="D38" s="12">
@@ -1907,15 +3624,58 @@
       <c r="J38" s="13">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="K38" s="27">
+        <v>572</v>
+      </c>
+      <c r="L38" s="23">
+        <v>13.3675</v>
+      </c>
+      <c r="M38" s="23">
+        <v>1.56077</v>
+      </c>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23">
+        <v>0</v>
+      </c>
+      <c r="P38" s="23">
+        <v>0.181979</v>
+      </c>
+      <c r="Q38" s="28">
+        <v>8.8339200000000007E-2</v>
+      </c>
+      <c r="R38" s="28">
+        <v>8.4805699999999998E-2</v>
+      </c>
+      <c r="S38" s="28">
+        <v>0.379859</v>
+      </c>
+      <c r="T38" s="28">
+        <v>2.8268600000000001E-2</v>
+      </c>
+      <c r="U38" s="28">
+        <v>1.23675E-2</v>
+      </c>
+      <c r="V38" s="28">
+        <v>0.114841</v>
+      </c>
+      <c r="W38" s="28">
+        <v>3.3568899999999999E-2</v>
+      </c>
+      <c r="X38" s="28">
+        <v>3.18021E-2</v>
+      </c>
+      <c r="Y38" s="28">
+        <v>0.22614799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="5">
         <v>4</v>
       </c>
       <c r="D39" s="12">
@@ -1939,15 +3699,60 @@
       <c r="J39" s="13">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="K39" s="27">
+        <v>10</v>
+      </c>
+      <c r="L39" s="23">
+        <v>9.1</v>
+      </c>
+      <c r="M39" s="23">
+        <v>1.9872000000000001</v>
+      </c>
+      <c r="N39" s="23">
+        <v>0</v>
+      </c>
+      <c r="O39" s="23">
+        <v>0</v>
+      </c>
+      <c r="P39" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="28">
+        <v>0</v>
+      </c>
+      <c r="R39" s="28">
+        <v>0</v>
+      </c>
+      <c r="S39" s="28">
+        <v>0.7</v>
+      </c>
+      <c r="T39" s="28">
+        <v>0</v>
+      </c>
+      <c r="U39" s="28">
+        <v>0</v>
+      </c>
+      <c r="V39" s="28">
+        <v>0</v>
+      </c>
+      <c r="W39" s="28">
+        <v>0</v>
+      </c>
+      <c r="X39" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y39" s="28">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="5">
         <v>0</v>
       </c>
       <c r="D40" s="12">
@@ -1968,18 +3773,53 @@
       <c r="I40" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J40" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="J40" s="16">
+        <v>0</v>
+      </c>
+      <c r="K40" s="27">
+        <v>0</v>
+      </c>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="28">
+        <v>0</v>
+      </c>
+      <c r="R40" s="28">
+        <v>0</v>
+      </c>
+      <c r="S40" s="28">
+        <v>0</v>
+      </c>
+      <c r="T40" s="28">
+        <v>0</v>
+      </c>
+      <c r="U40" s="28">
+        <v>0</v>
+      </c>
+      <c r="V40" s="28">
+        <v>0</v>
+      </c>
+      <c r="W40" s="28">
+        <v>0</v>
+      </c>
+      <c r="X40" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y40" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="5">
         <v>2</v>
       </c>
       <c r="D41" s="12">
@@ -2003,15 +3843,60 @@
       <c r="J41" s="13">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="K41" s="27">
+        <v>72</v>
+      </c>
+      <c r="L41" s="23">
+        <v>5.17143</v>
+      </c>
+      <c r="M41" s="23">
+        <v>0.51049999999999995</v>
+      </c>
+      <c r="N41" s="23">
+        <v>0</v>
+      </c>
+      <c r="O41" s="23">
+        <v>0</v>
+      </c>
+      <c r="P41" s="23">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="Q41" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="R41" s="28">
+        <v>0.157143</v>
+      </c>
+      <c r="S41" s="28">
+        <v>0.52857100000000001</v>
+      </c>
+      <c r="T41" s="28">
+        <v>4.2857100000000002E-2</v>
+      </c>
+      <c r="U41" s="28">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="V41" s="28">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="W41" s="28">
+        <v>1.42857E-2</v>
+      </c>
+      <c r="X41" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="28">
+        <v>0.12857099999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="5">
         <v>0</v>
       </c>
       <c r="D42" s="12">
@@ -2035,15 +3920,60 @@
       <c r="J42" s="13">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
+      <c r="K42" s="27">
+        <v>6</v>
+      </c>
+      <c r="L42" s="23">
+        <v>160.167</v>
+      </c>
+      <c r="M42" s="23">
+        <v>5.6916700000000002</v>
+      </c>
+      <c r="N42" s="23">
+        <v>0</v>
+      </c>
+      <c r="O42" s="23">
+        <v>0</v>
+      </c>
+      <c r="P42" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="28">
+        <v>0.83333299999999999</v>
+      </c>
+      <c r="R42" s="28">
+        <v>0</v>
+      </c>
+      <c r="S42" s="28">
+        <v>0</v>
+      </c>
+      <c r="T42" s="28">
+        <v>0</v>
+      </c>
+      <c r="U42" s="28">
+        <v>0</v>
+      </c>
+      <c r="V42" s="28">
+        <v>0</v>
+      </c>
+      <c r="W42" s="28">
+        <v>0</v>
+      </c>
+      <c r="X42" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="28">
+        <v>0.16666700000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="5">
         <v>2</v>
       </c>
       <c r="D43" s="12">
@@ -2064,18 +3994,63 @@
       <c r="I43" s="14">
         <v>35</v>
       </c>
-      <c r="J43" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="J43" s="16">
+        <v>0</v>
+      </c>
+      <c r="K43" s="27">
+        <v>5</v>
+      </c>
+      <c r="L43" s="23">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="M43" s="23">
+        <v>2.1682000000000001</v>
+      </c>
+      <c r="N43" s="23">
+        <v>0</v>
+      </c>
+      <c r="O43" s="23">
+        <v>0</v>
+      </c>
+      <c r="P43" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="R43" s="28">
+        <v>0</v>
+      </c>
+      <c r="S43" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="T43" s="28">
+        <v>0</v>
+      </c>
+      <c r="U43" s="28">
+        <v>0</v>
+      </c>
+      <c r="V43" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="W43" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="X43" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="5">
         <v>3</v>
       </c>
       <c r="D44" s="12">
@@ -2096,18 +4071,53 @@
       <c r="I44" s="14">
         <v>159</v>
       </c>
-      <c r="J44" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="J44" s="16">
+        <v>0</v>
+      </c>
+      <c r="K44" s="27">
+        <v>0</v>
+      </c>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="28">
+        <v>0</v>
+      </c>
+      <c r="R44" s="28">
+        <v>0</v>
+      </c>
+      <c r="S44" s="28">
+        <v>0</v>
+      </c>
+      <c r="T44" s="28">
+        <v>0</v>
+      </c>
+      <c r="U44" s="28">
+        <v>0</v>
+      </c>
+      <c r="V44" s="28">
+        <v>0</v>
+      </c>
+      <c r="W44" s="28">
+        <v>0</v>
+      </c>
+      <c r="X44" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="5">
         <v>5</v>
       </c>
       <c r="D45" s="12">
@@ -2131,18 +4141,61 @@
       <c r="J45" s="13">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="K45" s="27">
+        <v>1130</v>
+      </c>
+      <c r="L45" s="23">
+        <v>31.503799999999998</v>
+      </c>
+      <c r="M45" s="23">
+        <v>2.99464</v>
+      </c>
+      <c r="N45" s="23">
+        <v>0.23031299999999999</v>
+      </c>
+      <c r="O45" s="23">
+        <v>1.01609E-2</v>
+      </c>
+      <c r="P45" s="23"/>
+      <c r="Q45" s="28">
+        <v>0.117697</v>
+      </c>
+      <c r="R45" s="28">
+        <v>8.2133800000000007E-2</v>
+      </c>
+      <c r="S45" s="28">
+        <v>0.33615600000000001</v>
+      </c>
+      <c r="T45" s="28">
+        <v>3.97968E-2</v>
+      </c>
+      <c r="U45" s="28">
+        <v>1.9474999999999999E-2</v>
+      </c>
+      <c r="V45" s="28">
+        <v>0.136325</v>
+      </c>
+      <c r="W45" s="28">
+        <v>8.8061E-2</v>
+      </c>
+      <c r="X45" s="28">
+        <v>4.4877199999999999E-2</v>
+      </c>
+      <c r="Y45" s="28">
+        <v>0.13547799999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="5">
         <v>1</v>
       </c>
-      <c r="D46" s="16">
+      <c r="D46" s="17">
         <v>54430579</v>
       </c>
       <c r="E46" s="13">
@@ -2163,15 +4216,60 @@
       <c r="J46" s="13">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="K46" s="27">
+        <v>41</v>
+      </c>
+      <c r="L46" s="23">
+        <v>10.0488</v>
+      </c>
+      <c r="M46" s="23">
+        <v>1.60283</v>
+      </c>
+      <c r="N46" s="23">
+        <v>2.4390200000000001E-2</v>
+      </c>
+      <c r="O46" s="23">
+        <v>0</v>
+      </c>
+      <c r="P46" s="23">
+        <v>2.4390200000000001E-2</v>
+      </c>
+      <c r="Q46" s="28">
+        <v>0.121951</v>
+      </c>
+      <c r="R46" s="28">
+        <v>0.121951</v>
+      </c>
+      <c r="S46" s="28">
+        <v>0.48780499999999999</v>
+      </c>
+      <c r="T46" s="28">
+        <v>0</v>
+      </c>
+      <c r="U46" s="28">
+        <v>4.8780499999999997E-2</v>
+      </c>
+      <c r="V46" s="28">
+        <v>2.4390200000000001E-2</v>
+      </c>
+      <c r="W46" s="28">
+        <v>0</v>
+      </c>
+      <c r="X46" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="28">
+        <v>0.19512199999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="5">
         <v>5</v>
       </c>
       <c r="D47" s="12">
@@ -2192,18 +4290,53 @@
       <c r="I47" s="14">
         <v>72</v>
       </c>
-      <c r="J47" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
+      <c r="J47" s="16">
+        <v>0</v>
+      </c>
+      <c r="K47" s="27">
+        <v>0</v>
+      </c>
+      <c r="L47" s="23"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23"/>
+      <c r="Q47" s="28">
+        <v>0</v>
+      </c>
+      <c r="R47" s="28">
+        <v>0</v>
+      </c>
+      <c r="S47" s="28">
+        <v>0</v>
+      </c>
+      <c r="T47" s="28">
+        <v>0</v>
+      </c>
+      <c r="U47" s="28">
+        <v>0</v>
+      </c>
+      <c r="V47" s="28">
+        <v>0</v>
+      </c>
+      <c r="W47" s="28">
+        <v>0</v>
+      </c>
+      <c r="X47" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="5">
         <v>3</v>
       </c>
       <c r="D48" s="12">
@@ -2227,15 +4360,60 @@
       <c r="J48" s="13">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="K48" s="27">
+        <v>110</v>
+      </c>
+      <c r="L48" s="23">
+        <v>26.456299999999999</v>
+      </c>
+      <c r="M48" s="23">
+        <v>2.81711</v>
+      </c>
+      <c r="N48" s="23">
+        <v>1.9417500000000001E-2</v>
+      </c>
+      <c r="O48" s="23">
+        <v>0</v>
+      </c>
+      <c r="P48" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="28">
+        <v>0.106796</v>
+      </c>
+      <c r="R48" s="28">
+        <v>8.7378600000000001E-2</v>
+      </c>
+      <c r="S48" s="28">
+        <v>0.38834999999999997</v>
+      </c>
+      <c r="T48" s="28">
+        <v>2.9126200000000001E-2</v>
+      </c>
+      <c r="U48" s="28">
+        <v>0</v>
+      </c>
+      <c r="V48" s="28">
+        <v>1.9417500000000001E-2</v>
+      </c>
+      <c r="W48" s="28">
+        <v>3.8835000000000001E-2</v>
+      </c>
+      <c r="X48" s="28">
+        <v>3.8835000000000001E-2</v>
+      </c>
+      <c r="Y48" s="28">
+        <v>0.29126200000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="5">
         <v>2</v>
       </c>
       <c r="D49" s="12">
@@ -2259,15 +4437,60 @@
       <c r="J49" s="13">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="K49" s="27">
+        <v>25</v>
+      </c>
+      <c r="L49" s="23">
+        <v>5.76</v>
+      </c>
+      <c r="M49" s="23">
+        <v>0.84443999999999997</v>
+      </c>
+      <c r="N49" s="23">
+        <v>0</v>
+      </c>
+      <c r="O49" s="23">
+        <v>0</v>
+      </c>
+      <c r="P49" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="28">
+        <v>0.12</v>
+      </c>
+      <c r="R49" s="28">
+        <v>0.12</v>
+      </c>
+      <c r="S49" s="28">
+        <v>0.48</v>
+      </c>
+      <c r="T49" s="28">
+        <v>0.2</v>
+      </c>
+      <c r="U49" s="28">
+        <v>0</v>
+      </c>
+      <c r="V49" s="28">
+        <v>0.08</v>
+      </c>
+      <c r="W49" s="28">
+        <v>0</v>
+      </c>
+      <c r="X49" s="28">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="5">
         <v>1</v>
       </c>
       <c r="D50" s="12">
@@ -2291,15 +4514,60 @@
       <c r="J50" s="13">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
+      <c r="K50" s="27">
+        <v>400</v>
+      </c>
+      <c r="L50" s="23">
+        <v>14.9536</v>
+      </c>
+      <c r="M50" s="23">
+        <v>2.1058699999999999</v>
+      </c>
+      <c r="N50" s="23">
+        <v>9.79381E-2</v>
+      </c>
+      <c r="O50" s="23">
+        <v>0</v>
+      </c>
+      <c r="P50" s="23">
+        <v>7.7319600000000004E-3</v>
+      </c>
+      <c r="Q50" s="28">
+        <v>0.134021</v>
+      </c>
+      <c r="R50" s="28">
+        <v>0.14948500000000001</v>
+      </c>
+      <c r="S50" s="28">
+        <v>0.44587599999999999</v>
+      </c>
+      <c r="T50" s="28">
+        <v>2.0618600000000001E-2</v>
+      </c>
+      <c r="U50" s="28">
+        <v>1.5463899999999999E-2</v>
+      </c>
+      <c r="V50" s="28">
+        <v>0.113402</v>
+      </c>
+      <c r="W50" s="28">
+        <v>1.03093E-2</v>
+      </c>
+      <c r="X50" s="28">
+        <v>1.5463899999999999E-2</v>
+      </c>
+      <c r="Y50" s="28">
+        <v>9.5360799999999996E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="5">
         <v>3</v>
       </c>
       <c r="D51" s="12">
@@ -2323,15 +4591,60 @@
       <c r="J51" s="13">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+      <c r="K51" s="27">
+        <v>72</v>
+      </c>
+      <c r="L51" s="23">
+        <v>36.507199999999997</v>
+      </c>
+      <c r="M51" s="23">
+        <v>3.7694299999999998</v>
+      </c>
+      <c r="N51" s="23">
+        <v>5.7971000000000002E-2</v>
+      </c>
+      <c r="O51" s="23">
+        <v>0</v>
+      </c>
+      <c r="P51" s="23">
+        <v>8.6956500000000006E-2</v>
+      </c>
+      <c r="Q51" s="28">
+        <v>0.101449</v>
+      </c>
+      <c r="R51" s="28">
+        <v>7.2463799999999995E-2</v>
+      </c>
+      <c r="S51" s="28">
+        <v>0.34782600000000002</v>
+      </c>
+      <c r="T51" s="28">
+        <v>4.3478299999999998E-2</v>
+      </c>
+      <c r="U51" s="28">
+        <v>0</v>
+      </c>
+      <c r="V51" s="28">
+        <v>8.6956500000000006E-2</v>
+      </c>
+      <c r="W51" s="28">
+        <v>1.44928E-2</v>
+      </c>
+      <c r="X51" s="28">
+        <v>7.2463799999999995E-2</v>
+      </c>
+      <c r="Y51" s="28">
+        <v>0.26086999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="5">
         <v>4</v>
       </c>
       <c r="D52" s="12">
@@ -2355,15 +4668,60 @@
       <c r="J52" s="13">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+      <c r="K52" s="27">
+        <v>19</v>
+      </c>
+      <c r="L52" s="23">
+        <v>20.875</v>
+      </c>
+      <c r="M52" s="23">
+        <v>3.60825</v>
+      </c>
+      <c r="N52" s="23">
+        <v>6.25E-2</v>
+      </c>
+      <c r="O52" s="23">
+        <v>0</v>
+      </c>
+      <c r="P52" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="28">
+        <v>0.1875</v>
+      </c>
+      <c r="R52" s="28">
+        <v>6.25E-2</v>
+      </c>
+      <c r="S52" s="28">
+        <v>0.3125</v>
+      </c>
+      <c r="T52" s="28">
+        <v>0</v>
+      </c>
+      <c r="U52" s="28">
+        <v>0</v>
+      </c>
+      <c r="V52" s="28">
+        <v>6.25E-2</v>
+      </c>
+      <c r="W52" s="28">
+        <v>0</v>
+      </c>
+      <c r="X52" s="28">
+        <v>6.25E-2</v>
+      </c>
+      <c r="Y52" s="28">
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="5">
         <v>4</v>
       </c>
       <c r="D53" s="12">
@@ -2387,274 +4745,545 @@
       <c r="J53" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="K53" s="27">
+        <v>35</v>
+      </c>
+      <c r="L53" s="23">
+        <v>22.8857</v>
+      </c>
+      <c r="M53" s="23">
+        <v>3.2730600000000001</v>
+      </c>
+      <c r="N53" s="23">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="O53" s="23">
+        <v>0</v>
+      </c>
+      <c r="P53" s="23">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="Q53" s="28">
+        <v>0.114286</v>
+      </c>
+      <c r="R53" s="28">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="S53" s="28">
+        <v>0.45714300000000002</v>
+      </c>
+      <c r="T53" s="28">
+        <v>0</v>
+      </c>
+      <c r="U53" s="28">
+        <v>0</v>
+      </c>
+      <c r="V53" s="28">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="W53" s="28">
+        <v>8.5714299999999993E-2</v>
+      </c>
+      <c r="X53" s="28">
+        <v>5.7142900000000003E-2</v>
+      </c>
+      <c r="Y53" s="28">
+        <v>0.171429</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="23"/>
+      <c r="P54" s="23"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
         <v>53</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="3">
+      <c r="C55" s="7"/>
+      <c r="D55" s="12">
         <v>24772247</v>
       </c>
-      <c r="E55" s="4">
+      <c r="E55" s="13">
         <v>1323421.07</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F55" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="14">
         <v>4539</v>
       </c>
-      <c r="H55" s="5">
+      <c r="H55" s="14">
         <v>13</v>
       </c>
-      <c r="I55" s="5">
+      <c r="I55" s="14">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="J55" s="20">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K55" s="27">
+        <v>164</v>
+      </c>
+      <c r="L55" s="23">
+        <v>49.420699999999997</v>
+      </c>
+      <c r="M55" s="23">
+        <v>3.8695499999999998</v>
+      </c>
+      <c r="N55" s="23">
+        <v>0.54268300000000003</v>
+      </c>
+      <c r="O55" s="23">
+        <v>0.121951</v>
+      </c>
+      <c r="P55" s="23">
+        <v>1.21951E-2</v>
+      </c>
+      <c r="Q55" s="28">
+        <v>0.15853700000000001</v>
+      </c>
+      <c r="R55" s="28">
+        <v>0.18292700000000001</v>
+      </c>
+      <c r="S55" s="28">
+        <v>0.20122000000000001</v>
+      </c>
+      <c r="T55" s="28">
+        <v>7.92683E-2</v>
+      </c>
+      <c r="U55" s="28">
+        <v>2.4390200000000001E-2</v>
+      </c>
+      <c r="V55" s="28">
+        <v>0.13414599999999999</v>
+      </c>
+      <c r="W55" s="28">
+        <v>2.4390200000000001E-2</v>
+      </c>
+      <c r="X55" s="28">
+        <v>4.2682900000000003E-2</v>
+      </c>
+      <c r="Y55" s="28">
+        <v>0.15243899999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
         <v>54</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="3">
+      <c r="C56" s="7"/>
+      <c r="D56" s="12">
         <v>210867954</v>
       </c>
-      <c r="E56" s="4">
+      <c r="E56" s="13">
         <v>2055505.5</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="14">
         <v>1.3</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="14">
         <v>900</v>
       </c>
-      <c r="H56" s="5">
+      <c r="H56" s="14">
         <v>96</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I56" s="14">
         <v>106</v>
       </c>
-      <c r="J56" s="11">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="J56" s="20">
+        <v>1.26</v>
+      </c>
+      <c r="K56" s="27">
+        <v>173</v>
+      </c>
+      <c r="L56" s="23">
+        <v>30.9422</v>
+      </c>
+      <c r="M56" s="23">
+        <v>3.3571</v>
+      </c>
+      <c r="N56" s="23">
+        <v>0.32948</v>
+      </c>
+      <c r="O56" s="23">
+        <v>2.8901699999999999E-2</v>
+      </c>
+      <c r="P56" s="23">
+        <v>5.7803500000000001E-3</v>
+      </c>
+      <c r="Q56" s="28">
+        <v>0.104046</v>
+      </c>
+      <c r="R56" s="28">
+        <v>8.0924899999999994E-2</v>
+      </c>
+      <c r="S56" s="28">
+        <v>0.31791900000000001</v>
+      </c>
+      <c r="T56" s="28">
+        <v>8.6705199999999996E-2</v>
+      </c>
+      <c r="U56" s="28">
+        <v>2.31214E-2</v>
+      </c>
+      <c r="V56" s="28">
+        <v>0.20231199999999999</v>
+      </c>
+      <c r="W56" s="28">
+        <v>2.8901699999999999E-2</v>
+      </c>
+      <c r="X56" s="28">
+        <v>5.2023100000000003E-2</v>
+      </c>
+      <c r="Y56" s="28">
+        <v>0.104046</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
         <v>55</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="3">
+      <c r="C57" s="5"/>
+      <c r="D57" s="12">
         <v>127185332</v>
       </c>
-      <c r="E57" s="4">
+      <c r="E57" s="13">
         <v>4872136.95</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F57" s="14">
         <v>3.4</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="14">
         <v>5328</v>
       </c>
-      <c r="H57" s="5">
+      <c r="H57" s="14">
         <v>20</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I57" s="14">
         <v>9</v>
       </c>
-      <c r="J57" s="11">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="J57" s="20">
+        <v>3.21</v>
+      </c>
+      <c r="K57" s="27">
+        <v>197</v>
+      </c>
+      <c r="L57" s="23">
+        <v>41.198</v>
+      </c>
+      <c r="M57" s="23">
+        <v>3.6817099999999998</v>
+      </c>
+      <c r="N57" s="23">
+        <v>0.746193</v>
+      </c>
+      <c r="O57" s="23">
+        <v>0.22842599999999999</v>
+      </c>
+      <c r="P57" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="28">
+        <v>0.17766499999999999</v>
+      </c>
+      <c r="R57" s="28">
+        <v>0.18781700000000001</v>
+      </c>
+      <c r="S57" s="28">
+        <v>0.208122</v>
+      </c>
+      <c r="T57" s="28">
+        <v>4.0609100000000002E-2</v>
+      </c>
+      <c r="U57" s="28">
+        <v>3.5533000000000002E-2</v>
+      </c>
+      <c r="V57" s="28">
+        <v>9.1370599999999996E-2</v>
+      </c>
+      <c r="W57" s="28">
+        <v>5.0761399999999998E-3</v>
+      </c>
+      <c r="X57" s="28">
+        <v>3.5533000000000002E-2</v>
+      </c>
+      <c r="Y57" s="28">
+        <v>0.218274</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
         <v>56</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="B58" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="18">
+      <c r="C58" s="5"/>
+      <c r="D58" s="17">
         <v>66764851</v>
       </c>
-      <c r="E58" s="4">
+      <c r="E58" s="13">
         <v>2622433.96</v>
       </c>
-      <c r="F58" s="5">
+      <c r="F58" s="14">
         <v>1.7</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58" s="14">
         <v>4254</v>
       </c>
-      <c r="H58" s="5">
+      <c r="H58" s="14">
         <v>8</v>
       </c>
-      <c r="I58" s="5">
+      <c r="I58" s="14">
         <v>57</v>
       </c>
-      <c r="J58" s="11">
-        <v>3.21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="J58" s="20">
+        <v>1.66</v>
+      </c>
+      <c r="K58" s="27">
+        <v>171</v>
+      </c>
+      <c r="L58" s="23">
+        <v>121.40900000000001</v>
+      </c>
+      <c r="M58" s="23">
+        <v>5.4546999999999999</v>
+      </c>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23">
+        <v>0.23391799999999999</v>
+      </c>
+      <c r="P58" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="28">
+        <v>0.15789500000000001</v>
+      </c>
+      <c r="R58" s="28">
+        <v>0.204678</v>
+      </c>
+      <c r="S58" s="28">
+        <v>0.181287</v>
+      </c>
+      <c r="T58" s="28">
+        <v>9.9415199999999995E-2</v>
+      </c>
+      <c r="U58" s="28">
+        <v>1.7543900000000001E-2</v>
+      </c>
+      <c r="V58" s="28">
+        <v>0.146199</v>
+      </c>
+      <c r="W58" s="28">
+        <v>2.3391800000000001E-2</v>
+      </c>
+      <c r="X58" s="28">
+        <v>3.5087699999999999E-2</v>
+      </c>
+      <c r="Y58" s="28">
+        <v>0.13450300000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>57</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="18">
+      <c r="C59" s="5"/>
+      <c r="D59" s="17">
         <v>327921048</v>
       </c>
-      <c r="E59" s="4">
+      <c r="E59" s="13">
         <v>19390604</v>
       </c>
-      <c r="F59" s="5">
+      <c r="F59" s="14">
         <v>2.7</v>
       </c>
-      <c r="G59" s="5">
+      <c r="G59" s="14">
         <v>4255</v>
       </c>
-      <c r="H59" s="5">
+      <c r="H59" s="14">
         <v>16</v>
       </c>
-      <c r="I59" s="5">
+      <c r="I59" s="14">
         <v>121</v>
       </c>
-      <c r="J59" s="11">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
-      <c r="J60" s="11">
+      <c r="J59" s="20">
         <v>2.79</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="K59" s="27">
+        <v>168</v>
+      </c>
+      <c r="L59" s="23">
+        <v>102.488</v>
+      </c>
+      <c r="M59" s="23">
+        <v>7.7438799999999999</v>
+      </c>
+      <c r="N59" s="23"/>
+      <c r="O59" s="23">
+        <v>0.33132499999999998</v>
+      </c>
+      <c r="P59" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="28">
+        <v>0.210843</v>
+      </c>
+      <c r="R59" s="28">
+        <v>9.0361399999999995E-2</v>
+      </c>
+      <c r="S59" s="28">
+        <v>0.18072299999999999</v>
+      </c>
+      <c r="T59" s="28">
+        <v>0.15060200000000001</v>
+      </c>
+      <c r="U59" s="28">
+        <v>1.8072299999999999E-2</v>
+      </c>
+      <c r="V59" s="28">
+        <v>7.2289199999999998E-2</v>
+      </c>
+      <c r="W59" s="28">
+        <v>7.8313300000000002E-2</v>
+      </c>
+      <c r="X59" s="28">
+        <v>2.40964E-2</v>
+      </c>
+      <c r="Y59" s="28">
+        <v>0.17469899999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
         <v>101</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
         <v>102</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+    </row>
+    <row r="63" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
         <v>103</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="5"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="D63" s="14"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+    </row>
+    <row r="64" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
         <v>104</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="4">
         <v>105</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="4">
         <v>106</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="17"/>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C67" s="17"/>
-      <c r="D67" s="17"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="19"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C68" s="17"/>
-      <c r="D68" s="17"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="19"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="19"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="19"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="17"/>
-      <c r="D71" s="17"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>